<commit_message>
added basic files to repo hrd.xlsx sample data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE2D349-01EC-40D2-BAE3-916D9A40EE0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F49A7A5-0151-4907-BC96-CD9F90D56F12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -390,11 +390,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1111,7 +1111,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,20 +1149,20 @@
       <c r="A2" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>88</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1">
         <v>800</v>
       </c>
       <c r="E2" s="5">
-        <v>1</v>
+        <v>319</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="8" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1761,7 +1761,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1774,7 +1774,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1785,7 +1785,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
+      <c r="A2" s="19"/>
       <c r="B2" s="1" t="s">
         <v>58</v>
       </c>
@@ -1794,7 +1794,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="1" t="s">
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
added two files in repo
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B152B42-B27F-454D-839E-7E198C10B5C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C45F62C-675C-4EF9-A251-29F5DD85CEBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="90">
   <si>
     <t>halka</t>
   </si>
@@ -290,6 +290,9 @@
   </si>
   <si>
     <t>@jIt4hero</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=gmfMUZyoGXg</t>
   </si>
 </sst>
 </file>
@@ -1111,7 +1114,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,23 +1156,25 @@
         <v>88</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D2" s="1">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="E2" s="5">
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="8" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:6" s="12" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
+      <c r="A4" s="13" t="s">
+        <v>89</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1334,7 +1339,7 @@
   <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1761,7 +1766,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,7 +1959,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>